<commit_message>
MotivAcción Digital, instrumento para diagnosticar la motivación y preparación en transformación digital para mipymes
</commit_message>
<xml_diff>
--- a/MotivAccionDigital.xlsx
+++ b/MotivAccionDigital.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaperez/Documents/ANTEPROYECTO/MotivAcción Digital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0F5567-2602-664A-ADF7-27146DF6871C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06112B6-FCAE-2844-86A4-D66BAE382740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" tabRatio="874" firstSheet="1" activeTab="3" xr2:uid="{3D9F2410-914A-45BC-BADC-B7DDE18D258C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" tabRatio="874" activeTab="2" xr2:uid="{3D9F2410-914A-45BC-BADC-B7DDE18D258C}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="12" state="hidden" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="calculos" sheetId="10" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="154">
   <si>
     <t>Inicial</t>
   </si>
@@ -1240,6 +1239,7 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1279,7 +1279,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1757,18 +1756,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC86ECC-BD0F-4155-80EF-1F7C68008F57}">
   <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" customWidth="1"/>
-    <col min="5" max="5" width="33.5" customWidth="1"/>
-    <col min="6" max="6" width="60.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="44" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="62.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="60.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -2190,6 +2190,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="bw4BGpB1EFOB/cEvDo6ShG2U2vIznCyUwSEjvT84Va9YEAU4nv7QgApRoFhnJyjPuA8lmg6g7WkClLpOrkStnw==" saltValue="J+KAEcWUTTCMNI3b3YRi4A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2217,11 +2218,11 @@
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="str">
         <f>calculos!G10</f>
-        <v>Muy motivado</v>
+        <v>No motivado</v>
       </c>
       <c r="C1" t="str">
         <f>VLOOKUP(A1,Variables!N:O,2,0)</f>
-        <v>M</v>
+        <v>NM</v>
       </c>
       <c r="D1" s="11">
         <v>2</v>
@@ -2239,13 +2240,13 @@
     <row r="2" spans="1:7" ht="186" customHeight="1">
       <c r="A2" s="52" t="str">
         <f>A1</f>
-        <v>Muy motivado</v>
+        <v>No motivado</v>
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
       <c r="D2" s="54" t="str">
         <f>VLOOKUP(A1,Variables!U:V,2,0)</f>
-        <v>Tiene problemas que pueden llegar a poner en riesgo la operación de su negocio y que la transformación digital ayudaría a resolver, adicionalmente  considera relevante iniciar transformación digital en su empresa para apalancar sus proyectos a futuro y lograr las metas propuestas.</v>
+        <v>Hasta el momento no ha tenido problemas  con la operación actual de su negocio que la transformación digital ayudaría a resolver y no considera relevante iniciar transformación digital en su empresa  para apalancar sus proyectos a futuro y lograr las metas propuestas.</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -2262,56 +2263,52 @@
       <c r="B4"/>
       <c r="D4" s="29" t="str">
         <f>IFERROR(VLOOKUP(VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+D$1,Variables!$Q:$R,2,0),"")</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E4" s="30" t="str">
         <f>IFERROR(VLOOKUP(VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+E$1,Variables!$Q:$R,2,0),"")</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F4" s="31" t="str">
         <f>IFERROR(VLOOKUP(VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+F$1,Variables!$Q:$R,2,0),"")</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G4" s="32" t="str">
         <f>IFERROR(VLOOKUP(VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+G$1,Variables!$Q:$R,2,0),"")</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:7" ht="279" customHeight="1">
       <c r="A5" s="28" t="str">
         <f>IFERROR(IF(C1="NM","General",VLOOKUP(B5,'Diagnóstico de Preparación'!H:I,2,0)),IF('Diagnóstico de Preparación'!J6="Si","General",""))</f>
-        <v>Tecnologías y habilidades digitales</v>
+        <v>General</v>
       </c>
       <c r="B5" s="26">
         <v>1</v>
       </c>
-      <c r="C5" s="27" t="str">
+      <c r="C5" s="27" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A5,Variables!H:I,2,0))</f>
-        <v>M1</v>
+        <v>#N/A</v>
       </c>
       <c r="D5" s="51" t="str">
         <f>IF($C$1="NM",Matriz!C17,IFERROR(VLOOKUP($C$5,Matriz!$A:$F,VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+D$1,0),IF('Diagnóstico de Preparación'!J6="Si",Matriz!C17,"")))</f>
-        <v>Defina cómo considera que las herramientas tecnológicas del día a día pueden aportar para el desarrollo de su negocio. Por ejemplo: búsquedas en google, registro de información en Excel, uso de whatsapp Business, envío de correos electrónicos, crear documentos y carpetas para almacenar información en el computador, compartir archivos, entre otros.
-Evalúe si usted considera que usted o sus empleados deben conocer con mayor detalle cómo se utilizan estas herramientas.
-Si la respuesta es sí, defina si buscando material en internet puede autocapacitarse o si requiere que una persona o entidad brinde capacitaciones generales sobre uso de las Tecnologías de información y comunicación (TICs) y conocer sus beneficios.  Existen algunas aplicaciones disponibles en internet a las que puede acceder desde el celular para capacitarse en temática básica y conceptos introductorios como "Introducción a la informática y computación", "Introducción al paquete Office", "Guías de uso de computadores", entre otros. En Youtube hay algunos videos que pueden ser de su interés. Si definitivamente considera que no puede realizar la búsqueda en internet por su cuenta, apóyese en una persona que le pueda orientar.</v>
-      </c>
-      <c r="E5" s="50" t="str">
+        <v>Teniendo en cuenta que actualmente usted no ha tenido mayores problemas con la operación de su negocio que la transformación digital le ayudaría a resolver y tampoco considera relevante iniciar un proceso de transformación digital para sus proyectos a futuro en su empresa, actualmente no se recomienda realizar inversiones para iniciar un proceso de transformación digital dado que posiblemente no sería aprovechado o podrá verse como un gasto. En lugar de ello tenga en cuenta lo siguiente:
+La tecnología es un factor diferenciador para el mercado, se sugiere analizar el contexto de su empresa para que realmente evalúe si no requiere tecnología para volverse un mejor competidor y abarcar más negocios (más clientes, más ventas). Puede realizarlo así: Analice el comportamiento del sector de su negocio de los últimos 3 años, investigue como han sido las ventas, la participación en el mercado en su ciudad, en su barrio o sector, identifique si hay nuevos jugadores del mercado, si han llegado nuevos competidores y como están trabajando, busque cual es la proyección del mercado revisando noticias del sector de la economía donde su negocio participa principalmente, analice la promesa de valor de sus competidores, (identifique ventajas) de competidores de su mismo tamaño. Después de obtener este contexto se sugiere a que vuelva a diligenciar este instrumento, si su opinión y resultado no cambiaron, puede mantenerse al tanto de información de interés por medio de:
+https://www.innpulsacolombia.com/milab/nosotros
+https://www.portafolio.co/noticias-economicas/transformacion-digital
+https://gobiernodigital.mintic.gov.co/portal/Cursos/</v>
+      </c>
+      <c r="E5" s="50">
         <f>IF($C$1="NM",Matriz!D17,IFERROR(VLOOKUP($C$5,Matriz!$A:$F,VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+E$1,0),""))</f>
-        <v>Entienda en detalle su entorno, su negocio y sus clientes,  puede hacerse una idea por medio de las siguientes preguntas: ¿Quiénes son mis clientes?, ¿Qué servicio ofrece mi negocio?, ¿Cuales son mis principales competidores? . Con esto en mente, investigue si el uso de redes sociales para compartir contenido en medios digitales le es útil para incrementar sus ingresos, si es así, defina un plan de formación y capacítese en un nivel básico.
-Evalúe si herramientas de trabajo colaborativo como Google Docs, Office 365, Mensajería instantánea, le son de utilidad, si es así, fórmese usted y su equipo en conceptos básicos de seguridad para proteger su identidad en internet y brinde a su equipo de trabajo claridad acerca de los conceptos de Copyright y licencias. Investigue sobre conceptos y herramientas para proteger sus datos y dispositivos, explicando los riesgos existentes en los medios digitales. Algunos ejemplos de búsquedas que puede realizar en internet para este tema son: "Cómo crear contraseñas seguras", "Uso de antivirus en computadores", "Principales riesgos de seguridad en internet para mipymes", "Cómo proteger mi identidad en internet".
-Recuerde que estas herramientas no son útiles para todos los negocios, asegúrese de invertir su tiempo en iniciativas que realmente le permitan desarrollar su negocio y cumplir sus metas.</v>
-      </c>
-      <c r="F5" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
         <f>IF($C$1="NM",Matriz!E17,IFERROR(VLOOKUP($C$5,Matriz!$A:$F,VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+F$1,0),""))</f>
-        <v xml:space="preserve">
-Como su empresa se encuentra en un nivel de madurez competente en esta dimensión se recomienda fortalecer los conocimientos y capacidades sobre las TICs que ya se tienen por medio de capacitaciones a su equipo de trabajo. Puede ofrecer talleres generales por ejemplo sobre "Uso de Excel avanzado", "Pautar en redes sociales y estrategia de marca" entre otras capacitaciones especializadas sobre aspectos que se pueden requerir al adquirir nuevas tecnologías. Puede apoyarse por medio de convenios con plataformas de entrenamiento en línea, universidades, consultores independientes, instituciones educativas, cajas de compensación o la cámara de comercio de su ciudad.  Con un grupo de colaboradores puede iniciar un proceso de especialización sobre las nuevas tecnologías que se puedan requerir en el proceso de transformación. Otra alternativa que puede considerar es contratar a personal experto que se encargue de apoyarlo en funciones que requieran conocimiento especializado de software.
-Explore nuevas soluciones que existan en el mercado y le permitan incrementar sus ventas, por ejemplo: Rappi, Whatsapp Business u otras que no le impliquen desarrollos tecnológicos.
-Busque especializar el conocimiento del software que va  a poner a disposición del equipo de trabajo, puede  seleccionar un lider de excelencia. Prefiera entrenamiento gráfico y no manuales densos, incluya ejercicios prácticos de su día a día y con estos ejercicios fomente los entrenamientos requeridos en el personal de su empresa.</v>
-      </c>
-      <c r="G5" s="12" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
         <f>IF($C$1="NM",Matriz!F17,IFERROR(VLOOKUP($C$5,Matriz!$A:$F,VLOOKUP($A5,'Diagnóstico de Preparación'!$B:$F,5,0)+G$1,0),""))</f>
-        <v>La transformación digital puede involucrar adquirir software o hardware  que requiere conocimientos digitales especializados, como su empresa se encuentra en un nivel de madurez avanzado en esta dimensión puede considerar construir un "Centro de Excelencia" con los empleados expertos en algunos temas, con ellos puede planear un programa de formación general, ejecutarlo y medir el retorno de inversión. También puede vincular paulatinamente personal experto que cuente con conocimiento especializado en los temas y aplicaciones que está adquiriendo.
-Contrate expertos o tercerice actividades de soporte especializado, seguridad informática y prepárese ante los riesgos cibernéticos. Actualícese frecuentemente en cuanto a tendencias, herramientas, dispositivos y riesgos de habilitar sus procesos de forma distribuida o en la nube. Puede explorar soluciones de inteligencia artificial ante problemas recurrentes de su empresa.</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16">
@@ -2325,359 +2322,253 @@
       <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:7" ht="21">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="38" t="str">
         <f>IF($C$1="NM","",IFERROR(VLOOKUP(VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+D$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E8" s="39" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+E$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F8" s="40" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+F$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G8" s="41" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+G$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:7" ht="409" customHeight="1">
       <c r="A9" s="26" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(B9,'Diagnóstico de Preparación'!H:I,2,0),""))</f>
-        <v>Comunicaciones y canales de venta</v>
+        <v/>
       </c>
       <c r="B9" s="26">
         <v>2</v>
       </c>
-      <c r="C9" s="27" t="str">
+      <c r="C9" s="27" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A9,Variables!H:I,2,0))</f>
-        <v>M2</v>
+        <v>#N/A</v>
       </c>
       <c r="D9" s="12" t="str">
         <f>IFERROR(VLOOKUP($C9,Matriz!$A:$F,VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+D$1,0),"")</f>
-        <v>Es fundamental que empiece a conocer sus clientes, ellos son quienes deben permitirle establecer qué cambios debe realizar en su proceso de venta, para esto, se sugiere que defina un mecanismo sencillo para empezar a recibir comentarios, por ejemplo: una encuesta al finalizar cada venta (presencial, por whatsapp), telefónica, inicialmente puede ser a través un formulario impreso. Empiece a consolidar la información para que pueda definir iniciativas que le aporten al desarrollo de su negocio.
-Adicionalmente, inicie la promoción de productos y servicios a través de por lo menos, un medio digital, por ejemplo a través de redes sociales como Facebook, Instagram, Youtube, LinkedIn -y similares-, sistemas de mensajería comoWhatsApp o Telegram.</v>
+        <v/>
       </c>
       <c r="E9" s="12" t="str">
         <f>IFERROR(VLOOKUP($C9,Matriz!$A:$F,VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+E$1,0),"")</f>
-        <v xml:space="preserve">Se recomienda recibir directamente comentarios de los clientes y observar sus acciones para identificar necedidades, deseos y expectativas. En este nivel de madurez para su empresa, la interacción puede ser en el mismo momento en que el cliente adquiere los productos y servicios y no solo al final del proceso. Registre los comentarios de los clientes en algún documento o sistema que le permita consolidar la información. Ejemplo Excel, Microsoft Forms, Encuestas de Google, entre otras.
-Defina las iniciativas que le van a permitir facilitar la comunicación con sus clientes y el acceso a sus productos / servicios. Esto lo puede identificar con base en las recomendaciones que sus clientes le realicen sobre aspectos que les gustaría que su empresa ofreciera.
-Ejemplos de iniciativas: 
-Involucrar dos o más canales digitales adicionales para lograr acceder a más clientes, incrementar su presencia digital por ejemplo a través de una página web de la empresa o sumándose a un sitio de comercio en línea (Marketplace). Ejemplos de algunos marketplaces gratuitos pueden ser: Facebook marketplace, Mercadolibre, Linio, OLX, Whatsapp business, Rappi
-Para esto es necesario tomar fotos de buena calidad de los productos y establecer cierta periodicidad para actualizar los anuncios, es importante que sus ofertas por medios digitales se encuentren actualizadas con frecuencia.
-Otras iniciativas: Diversificación de medios de pago, posibilidad de recibir pagos por medio de transferencias bancarias o códigos QR, tarjetas débito y crédito, además del efectivo. Agendamiento de pedidos en línea, planificación de horas de entrega, u otros diferenciales que pueda incluir justo en el momento en el que está cerrando una venta.
-Priorice 2 de sus iniciativas, se sugiere que inicie por aquellas que tengan menos complejidad para que pueda evaluar el impacto rapidamente que trae al negocio, en otras palabras, que le permita identificar si esto aportará significativamente a su crecimiento.
-</v>
+        <v/>
       </c>
       <c r="F9" s="12" t="str">
         <f>IFERROR(VLOOKUP($C9,Matriz!$A:$F,VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+F$1,0),"")</f>
-        <v xml:space="preserve">Es recomendable que las interacciones con los clientes sean durante el proceso de compra o de uso de un servicio de manera que permita visualizar su experienca para identificar necesidades no cubiertas y calificar su experiencia, trabaje en evolucionar la identificación de aspectos positivos y por mejorar directamente de sus clientes. 
-Algunos ejemplos pueden ser visitas incógnitas a los puntos de venta, llamadas a las líneas de atención, intentar ejecutar un proceso simulando ser el cliente. En este punto es valioso iniciar métricas de satisfacción. Establezca alguna métrica para recibir en cada compra una valoración del proceso y pueda utilizarlo a futuro para establecer acciones de mejora. Empiece a medir la efectividad de los canales establecidos, e incorpore los resultados dentro de su proceso de análisis.
-Esto debe tener como resultado, la inclusión de nuevos canales constantemente, la evolución de los existentes o la eliminación de aquellos que no generen valor.
-Adicionalmente, en este nivel de madurez se recomienda que ofrezca una experiencia unificada y consistente para los clientes, por medio de las interacciones de los canales digitales y tomado como base las métricas que se hayan logrado generar de procesos de venta o uso de servicios por medios digitales y no digitales. De esta forma, la experiencia de utilizar o consumir sus productos como empresa resultará consistente y no aislada por cada canal.
-</v>
+        <v/>
       </c>
       <c r="G9" s="12" t="str">
         <f>IFERROR(VLOOKUP($C9,Matriz!$A:$F,VLOOKUP(B9,'Diagnóstico de Preparación'!E:F,2,0)+G$1,0),"")</f>
-        <v>En este nivel de madurez es importante sistematizar las interacciones de los clientes mediante un proceso que permita tomar en cuenta sus recomendaciones, calificaciones y utilizarlas como insumo para mejorar o generar nuevas soluciones o productos, así como elevar la capacidad de medir el retorno de inversión de estos.
-Por ejemplo antes de lanzar un nuevo producto o servicio al mercado se sugiere tomar una base de clientes diversos que aporten ideas, comentarios y desde su experiencia permitan enriquecer la creación de esos nuevos productos. Se pueden generar espacios presenciales o virtuales motivados con con incentivos (desayunos, souvenirs, etc). Puede considerar la creación de laboratorios donde se explore la creatividad y se puedan generar ideas novedosas de productos o servicios a ofrecer por su empresa.</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="22" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+D$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E12" s="23" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+E$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F12" s="24" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+F$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G12" s="25" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+G$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7" ht="408.75" customHeight="1">
       <c r="A13" s="10" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(B13,'Diagnóstico de Preparación'!H:I,2,0),""))</f>
-        <v>Organización y personas</v>
+        <v/>
       </c>
       <c r="B13" s="10">
         <v>3</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A13,Variables!H:I,2,0))</f>
-        <v>M3</v>
+        <v>#N/A</v>
       </c>
       <c r="D13" s="12" t="str">
         <f>IFERROR(VLOOKUP($C13,Matriz!$A:$F,VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+D$1,0),"")</f>
-        <v xml:space="preserve">La tecnología por sí sola no permite alcanzar resultados, la manera en la que las personas utilizan las herramientas es lo que realmente permite la generación de valor, es por esto que es importante que identifique qué tan preparado está usted y su equipo para cambiar la manera de operar su negocio dando entrada a la tecnología en las actividades del día a día.
-Para esto se recomienda identificar en su día a día qué equipos de trabajo no utilizan tecnologías digitales en sus actividades diarias y mantienen formas de trabajo tradicionales, para establecerlos como objetivo y por medio de un  esquema de comunicación  mostrar cómo la tecnología ayudará a hacer su trabajo mejor y más rápido. 
-Es relevante incluir talleres con ejemplos específicos de tareas que antes se realizaban en mayor tiempo o que ni siquiera eran posibles, y mostrar visualmente cómo serían viables empleando la nueva tecnología.
-1. Realice  acercamientos con las personas de su equipo de trabajo, indague sobre cuales son las motivaciones que tienen para usar o no usar la tecnología. Esto le permitirá identificar algunos prejuicios o bloqueantes que deba atacar en primer momento. 
-2. Elabore un Plan de formación, indagando a un mayor nivel de detalle con su equipo de trabajo para identificar a quienes y sobre que temas se deben formar, cada persona puede requerir un plan distinto teniendo en cuenta sus necesidades y competencias.
-La formación debe contemplar  el entendimiento de uso de la solución digital y las habilidades técnicas y blandas para sacarle provecho a dicha solución.
-3. Brinde acompañamiento, permítale a su equipo de trabajo ser parte activa del proceso de transformación, incentive y reconozca los logros en las personas que apoyen el ejercicio de movilización con, por ejemplo, souvenirs, recononocimiento público, salario emocional.
-4. Inicie una medición para llevar un control sobre la efectividad de los planes de formación. </v>
+        <v/>
       </c>
       <c r="E13" s="12" t="str">
         <f>IFERROR(VLOOKUP($C13,Matriz!$A:$F,VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+E$1,0),"")</f>
-        <v xml:space="preserve">Se recomienda que identifique una persona o equipo de trabajo que colabore con los demás integrantes en cuanto a  nuevas formas de hacer las cosas. Estas personas se conocen como promotores que propician mentalidad de crecimiento.
-Fomente el aprendizaje y genere un ambiente de apoyo cuando existan problemas y desafíos durante la implementación de nuevas tecnologías. 
-Mantenga una comunicación fluida y ponga al alcance de los usuarios recursos de ayuda, ejemplos de ello son sesiones de mensajería en chat corporativos, Microsoft Teams, google meets, grupos de whatsapp, sesiones presenciales y virtuales para socializar experiencias y aclarar dudas en la implementación de nueva tecnología.
-Implemente  espacios para socializar con su equipo de trabajo los finales  de un proyecto, resultados, cambios, beneficios y permìtales socializar en la manera en que cada persona desde su rol se verá beneficiada.
-Evalúe si su modelo de negocio le permite incorporar prácticas laborales alineadas a las nuevas tendencias de las empresas digitales, y qué tanto valor le genera esto a sus empleados, por ejemplo: trabajo híbrido o remoto, flexibilidad de horarios, trabajo orientado a resultados y no al tiempo invertido presencial. (Tenga en cuenta que no todos los negocios pueden incluir estas prácticas)
-</v>
+        <v/>
       </c>
       <c r="F13" s="12" t="str">
         <f>IFERROR(VLOOKUP($C13,Matriz!$A:$F,VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+F$1,0),"")</f>
-        <v xml:space="preserve">Identifique las cualidades y capacidades que requiere que tenga su equipo de trabajo para el proceso de transformación, evalúe a su equipo existente y genere planes que le permitan desarrollar y/o elevar estas capacidades, algunas tácticas para esto son:
-1. Genere espacios para hacer feedback (Consiste en la manifestación de una opinión y demostración de un punto de vista. El feedback es utilizado, por ejemplo, para evaluar a una persona, una empresa, un producto o un servicio) donde se establezcan compromisos claros de desarrollo de cada empleado.
-2. Genere dinámicas de juegos de roles: esto usualmente permite que las personas se auto evalúen e identifiquen sus oportunidades de mejora.
-3. Realice entrevistas a personas del equipo de trabajo para conocer en qué estado se encuentran las relaciones y el trabajo en equipo. (Se conoce como medir el clima laboral)
-4. Genere dinámicas que permitan el desarrollo de la confianza, sospeche cuando todo lo que le cuente su equipo de trabajo sea positivo.
-Cuando un colaborador tiene brechas significativas, debe evaluar la pertinencia de su continuidad en el negocio.
-En este nivel es importante que realice mediciones, mediante seguimientos que permitan entender lo que siente su equipo de trabajo. Genere indicadores que permitan tener alertas para hacer ajustes en la estrategia de formación. Ejemplos de indicadores pueden ser: Procesos de la empresa impactados por el plan de capacitación, satisfacción de las partes interesadas con el plan de formación. 
-Genere refuerzos e incentivos sobre comportamientos deseados por su equipo de trabajo, recuerde que la meta es que los comportamientos deseados  permanezcan en el tiempo.
-</v>
+        <v/>
       </c>
       <c r="G13" s="12" t="str">
         <f>IFERROR(VLOOKUP($C13,Matriz!$A:$F,VLOOKUP(B13,'Diagnóstico de Preparación'!E:F,2,0)+G$1,0),"")</f>
-        <v xml:space="preserve">Defina mecanismos que le permitan identificar si la cultura que requiere su negocio es un hábito en el día a día, la manera más sencilla de identificarlo, es que nuevos integrantes resalten esa cualidad de su equipo de trabajo cuando llevan corto tiempo en su negocio.
-Periódicamente, realice capacitaciones y/o dinámicas que le permitan reforzar los comportamientos característica y hábitos que usted definió como habilitadores para la evolución digital continua de su empresa. Continúe realizando mediciones sobre la satisfacción de su equipo de trabajo. Genere refuerzos e incentivos sobre comportamientos deseados por su equipo de trabajo, recuerde que la meta es que los comportamientos deseados  permanezcan en el tiempo. 
-</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="67"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="22" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+D$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E16" s="23" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+E$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F16" s="24" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+F$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G16" s="25" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+G$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:7" ht="409.5" customHeight="1">
       <c r="A17" s="10" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(B17,'Diagnóstico de Preparación'!H:I,2,0),""))</f>
-        <v>Estrategia y transformación digital</v>
+        <v/>
       </c>
       <c r="B17" s="10">
         <v>4</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A17,Variables!H:I,2,0))</f>
-        <v>M4</v>
+        <v>#N/A</v>
       </c>
       <c r="D17" s="12" t="str">
         <f>IFERROR(VLOOKUP($C17,Matriz!$A:$F,VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+D$1,0),"")</f>
-        <v>Esta dimensión es transversal para todos los niveles de madurez. Por favor tenga en cuenta lo siguiente:
-Para conocer donde se encuentra actualmente su empresa y  cual es su propuesta de valor se sugiere utilizar el Modelo Canva, el cual consiste en una plantilla de 9 secciones para identificar los elementos más relevantes de su empresa, utilícelo como punto de partida. En este sitio web se encuentra información que puede resultar útil: https://blog.hubspot.es/sales/modelo-canvas. Con esto en mente, tenga en cuenta lo siguiente:
-La estrategia es la base para construir una ruta y encaminar correctamente los esfuerzos en transformación digital. Es importante que revise su estrategia por medio de los siguientes pasos:
-1. Analice el comportamiento del sector de su negocio de los últimos 3 años, investigue como han sido las ventas, la participación en el mercado en su ciudad, en su barrio o sector, identifique si hay nuevos jugadores del mercado, si han llegado nuevos competidores y como están trabajando, busque cual es la proyección del mercado revisando noticias del sector de la economía donde su negocio participa principalmente, analice la promesa de valor de sus competidores, (identifique ventajas) de competidores de su mismo tamaño. Con esto responde la pregunta : Dónde está ubicado?
-2. Identifique en donde quiere estar
-Como ya hizo un ejercicio previo de ver el mercado y sumado a su experiencia en el gremio y en su sector, póngase una o varias metas en un horizonte de tiempo de máximo 3 años. (ejemplos: Incrementar la utilidad del negocio, expandirse geográficamente, diversificar la oferta,). Con esto en mente genere una lluvia de ideas de iniciativas que se pueden realizar para cada objetivo, por ejemplo: Generar ventas por medio de canales digitales, Implementar un CRM (Customer Relationship Management) para segmentar adecuadamente los clientes, Automatizar un proceso, entre otras. A lo largo de la presente matriz de recomendaciones encontrará ejemplos de iniciativas que le permitirán iniciar un proceso de transformación alineado con lo que usted como empresario desea para su negocio.
-3. Enfóquese, seleccione de todas iniciativas cuales considera viables en el lapso de tiempo definido (3 años). Puede utilizar una técnica de impacto vs esfuerzo, se encuentra información relacionada en https://miro.com/es/plantillas/matriz-de-esfuerzo-impacto/, clasifique cada iniciativa en nivel de impacto: Alto o Bajo y nivel de esfuerzo Alto o Bajo). Lo que esté en el cuadrante de Alto impacto con bajo esfuerzo, va primero. Las iniciativas del cuadrante Alto impacto Alto esfuerzo puede ir en segundo lugar.
-Reconsidere si alcanza en el tiempo establecido. Las iniciativas que tienen alto esfuerzo y bajo impacto descártelas. Al final del ejercicio tendrá un listado de iniciativas que lo pueden ayudar a alcanzar sus objetivos.</v>
+        <v/>
       </c>
       <c r="E17" s="12" t="str">
         <f>IFERROR(VLOOKUP($C17,Matriz!$A:$F,VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+E$1,0),"")</f>
-        <v>Esta dimensión es transversal para todos los niveles de madurez. Por favor tenga en cuenta lo siguiente:
-Para conocer donde se encuentra actualmente su empresa y  cual es su propuesta de valor se sugiere utilizar el Modelo Canva, el cual consiste en una plantilla de 9 secciones para identificar los elementos más relevantes de su empresa, utilícelo como punto de partida. En este sitio web se encuentra información que puede resultar útil: https://blog.hubspot.es/sales/modelo-canvas. Con esto en mente, tenga en cuenta lo siguiente:
-La estrategia es la base para construir una ruta y encaminar correctamente los esfuerzos en transformación digital. Es importante que revise su estrategia por medio de los siguientes pasos:
-1. Analice el comportamiento del sector de su negocio de los últimos 3 años, investigue como han sido las ventas, la participación en el mercado en su ciudad, en su barrio o sector, identifique si hay nuevos jugadores del mercado, si han llegado nuevos competidores y como están trabajando, busque cual es la proyección del mercado revisando noticias del sector de la economía donde su negocio participa principalmente, analice la promesa de valor de sus competidores, (identifique ventajas) de competidores de su mismo tamaño. Con esto responde la pregunta : Dónde está ubicado?
-2. Identifique en donde quiere estar
-Como ya hizo un ejercicio previo de ver el mercado y sumado a su experiencia en el gremio y en su sector, póngase una o varias metas en un horizonte de tiempo de máximo 3 años. (ejemplos: Incrementar la utilidad del negocio, expandirse geográficamente, diversificar la oferta,). Con esto en mente genere una lluvia de ideas de iniciativas que se pueden realizar para cada objetivo, por ejemplo: Generar ventas por medio de canales digitales, Implementar un CRM (Customer Relationship Management) para segmentar adecuadamente los clientes, Automatizar un proceso, entre otras. A lo largo de la presente matriz de recomendaciones encontrará ejemplos de iniciativas que le permitirán iniciar un proceso de transformación alineado con lo que usted como empresario desea para su negocio.
-3. Enfóquese, seleccione de todas iniciativas cuales considera viables en el lapso de tiempo definido (3 años). Puede utilizar una técnica de impacto vs esfuerzo, se encuentra información relacionada en https://miro.com/es/plantillas/matriz-de-esfuerzo-impacto/, clasifique cada iniciativa en nivel de impacto: Alto o Bajo y nivel de esfuerzo Alto o Bajo). Lo que esté en el cuadrante de Alto impacto con bajo esfuerzo, va primero. Las iniciativas del cuadrante Alto impacto Alto esfuerzo puede ir en segundo lugar.
-Reconsidere si alcanza en el tiempo establecido. Las iniciativas que tienen alto esfuerzo y bajo impacto descártelas. Al final del ejercicio tendrá un listado de iniciativas que lo pueden ayudar a alcanzar sus objetivos.</v>
+        <v/>
       </c>
       <c r="F17" s="12" t="str">
         <f>IFERROR(VLOOKUP($C17,Matriz!$A:$F,VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+F$1,0),"")</f>
-        <v>Esta dimensión es transversal para todos los niveles de madurez. Por favor tenga en cuenta lo siguiente:
-Para conocer donde se encuentra actualmente su empresa y  cual es su propuesta de valor se sugiere utilizar el Modelo Canva, el cual consiste en una plantilla de 9 secciones para identificar los elementos más relevantes de su empresa, utilícelo como punto de partida. En este sitio web se encuentra información que puede resultar útil: https://blog.hubspot.es/sales/modelo-canvas. Con esto en mente, tenga en cuenta lo siguiente:
-La estrategia es la base para construir una ruta y encaminar correctamente los esfuerzos en transformación digital. Es importante que revise su estrategia por medio de los siguientes pasos:
-1. Analice el comportamiento del sector de su negocio de los últimos 3 años, investigue como han sido las ventas, la participación en el mercado en su ciudad, en su barrio o sector, identifique si hay nuevos jugadores del mercado, si han llegado nuevos competidores y como están trabajando, busque cual es la proyección del mercado revisando noticias del sector de la economía donde su negocio participa principalmente, analice la promesa de valor de sus competidores, (identifique ventajas) de competidores de su mismo tamaño. Con esto responde la pregunta : Dónde está ubicado?
-2. Identifique en donde quiere estar
-Como ya hizo un ejercicio previo de ver el mercado y sumado a su experiencia en el gremio y en su sector, póngase una o varias metas en un horizonte de tiempo de máximo 3 años. (ejemplos: Incrementar la utilidad del negocio, expandirse geográficamente, diversificar la oferta,). Con esto en mente genere una lluvia de ideas de iniciativas que se pueden realizar para cada objetivo, por ejemplo: Generar ventas por medio de canales digitales, Implementar un CRM (Customer Relationship Management) para segmentar adecuadamente los clientes, Automatizar un proceso, entre otras. A lo largo de la presente matriz de recomendaciones encontrará ejemplos de iniciativas que le permitirán iniciar un proceso de transformación alineado con lo que usted como empresario desea para su negocio.
-3. Enfóquese, seleccione de todas iniciativas cuales considera viables en el lapso de tiempo definido (3 años). Puede utilizar una técnica de impacto vs esfuerzo, se encuentra información relacionada en https://miro.com/es/plantillas/matriz-de-esfuerzo-impacto/, clasifique cada iniciativa en nivel de impacto: Alto o Bajo y nivel de esfuerzo Alto o Bajo). Lo que esté en el cuadrante de Alto impacto con bajo esfuerzo, va primero. Las iniciativas del cuadrante Alto impacto Alto esfuerzo puede ir en segundo lugar.
-Reconsidere si alcanza en el tiempo establecido. Las iniciativas que tienen alto esfuerzo y bajo impacto descártelas. Al final del ejercicio tendrá un listado de iniciativas que lo pueden ayudar a alcanzar sus objetivos.</v>
+        <v/>
       </c>
       <c r="G17" s="12" t="str">
         <f>IFERROR(VLOOKUP($C17,Matriz!$A:$F,VLOOKUP(B17,'Diagnóstico de Preparación'!E:F,2,0)+G$1,0),"")</f>
-        <v>Esta dimensión es transversal para todos los niveles de madurez. Por favor tenga en cuenta lo siguiente:
-Para conocer donde se encuentra actualmente su empresa y  cual es su propuesta de valor se sugiere utilizar el Modelo Canva, el cual consiste en una plantilla de 9 secciones para identificar los elementos más relevantes de su empresa, utilícelo como punto de partida. En este sitio web se encuentra información que puede resultar útil: https://blog.hubspot.es/sales/modelo-canvas. Con esto en mente, tenga en cuenta lo siguiente:
-La estrategia es la base para construir una ruta y encaminar correctamente los esfuerzos en transformación digital. Es importante que revise su estrategia por medio de los siguientes pasos:
-1. Analice el comportamiento del sector de su negocio de los últimos 3 años, investigue como han sido las ventas, la participación en el mercado en su ciudad, en su barrio o sector, identifique si hay nuevos jugadores del mercado, si han llegado nuevos competidores y como están trabajando, busque cual es la proyección del mercado revisando noticias del sector de la economía donde su negocio participa principalmente, analice la promesa de valor de sus competidores, (identifique ventajas) de competidores de su mismo tamaño. Con esto responde la pregunta : Dónde está ubicado?
-2. Identifique en donde quiere estar
-Como ya hizo un ejercicio previo de ver el mercado y sumado a su experiencia en el gremio y en su sector, póngase una o varias metas en un horizonte de tiempo de máximo 3 años. (ejemplos: Incrementar la utilidad del negocio, expandirse geográficamente, diversificar la oferta,). Con esto en mente genere una lluvia de ideas de iniciativas que se pueden realizar para cada objetivo, por ejemplo: Generar ventas por medio de canales digitales, Implementar un CRM (Customer Relationship Management) para segmentar adecuadamente los clientes, Automatizar un proceso, entre otras. A lo largo de la presente matriz de recomendaciones encontrará ejemplos de iniciativas que le permitirán iniciar un proceso de transformación alineado con lo que usted como empresario desea para su negocio.
-3. Enfóquese, seleccione de todas iniciativas cuales considera viables en el lapso de tiempo definido (3 años). Puede utilizar una técnica de impacto vs esfuerzo, se encuentra información relacionada en https://miro.com/es/plantillas/matriz-de-esfuerzo-impacto/, clasifique cada iniciativa en nivel de impacto: Alto o Bajo y nivel de esfuerzo Alto o Bajo). Lo que esté en el cuadrante de Alto impacto con bajo esfuerzo, va primero. Las iniciativas del cuadrante Alto impacto Alto esfuerzo puede ir en segundo lugar.
-Reconsidere si alcanza en el tiempo establecido. Las iniciativas que tienen alto esfuerzo y bajo impacto descártelas. Al final del ejercicio tendrá un listado de iniciativas que lo pueden ayudar a alcanzar sus objetivos.</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="38" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+D$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E20" s="39" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+E$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F20" s="40" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+F$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G20" s="41" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+G$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:7" ht="379" customHeight="1">
       <c r="A21" s="10" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(B21,'Diagnóstico de Preparación'!H:I,2,0),""))</f>
-        <v>Datos y analítica</v>
+        <v/>
       </c>
       <c r="B21" s="10">
         <v>5</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A21,Variables!H:I,2,0))</f>
-        <v>M5</v>
+        <v>#N/A</v>
       </c>
       <c r="D21" s="12" t="str">
         <f>IFERROR(VLOOKUP($C21,Matriz!$A:$F,VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+D$1,0),"")</f>
-        <v>Cuando se está en una etapa inicial se debe identificar los elementos a "medir" con base en las necesidades actuales de su negocio. 
-Pasos:
-1.Defina qué es lo que quiere medir. Es decir, genere preguntas que quisiera responder con datos.
-2.Confirme si cuenta con la información para poder generar la medición, en caso de que no sea así, evalúe si es sencillo empezar a recolectar los datos necesarios, si es así, avance al siguiente paso, si no, coloque el indicador en lista de espera o deseables.
-3. Priorice los indicadores, seleccione 3 o máximo 5 indicadores
-Inicie la medición con base en lo que tiene. Por ejemplo, hojas de cálculo en excel, información en papel, y saque las medidas de las preguntas que desea responder.
-Recomendación: no se enfoque en tener datos perfectos si no es necesario, para iniciar puede convivir con algún margen de error en la exactitud de los datos, mientras va desarrollando la capacidad, va a ir identificando en dónde requiere exactitud y dónde no.
-Ejemplo: Usted tiene un negocio de venta de empanadas, y requiere saber cuánta harina de maiz se gasta por mes (para iniciar no se requiere el peso exacto, puede trabajar en sus indicadores por paquetes o libras de harina en múltiplos de 10). Ejemplo de indicadores: cuántas empanadas se venden en un fin de semana?  cuánta ganancia deja cada empanada?
-Recuerde confirmar si cuenta con la información  necesaria por ejemplo, no ha tomado el historial de cuanto material (harina) se gasta en hacer cierta cantidad de empanadas, entonces debe empezar a registar esa información para saber si lo puede o no medir."</v>
+        <v/>
       </c>
       <c r="E21" s="12" t="str">
         <f>IFERROR(VLOOKUP($C21,Matriz!$A:$F,VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+E$1,0),"")</f>
-        <v>En esta etapa se recomienda evaluar los indicadores o las mediciones existentes con base en las siguientes preguntas/sugerencias:
-1. ¿Los indicadores que estoy generando siguen siendo valiosos para el desarrollo de mi negocio?, si la respuesta es sí, garantice que tiene datos históricos que le permitan compararse para trazarse metas que lo lleven a un siguiente nivel, así mismo, trabaje en garantizar la calidad de estos datos. Si la respuesta es no, deseche el indicador.
-2. Revise su lista de espera o de  indicadores deseables, evalúe cuál es el siguiente paquete (máximo 5) que debe empezar a medir para desarrollar su negocio. Defina un mecanismo simple que le permita iniciar a recolectar los datos que necesite.
-Ejemplo de las empanadas: Cuántas empanadas hago al día, cuánta sal me gasto en un mes, etc. Nivel de productividad, cuánto tiempo se demora haciendo una empanada, en cuánto tiempo vendo una empanada, utilidad de cada empanada.
-Ejemplo, ver si tengo la info para el de los materiales. O cuánto me demora haciendo una empanada, arranco con lo que tengo y lo que puedo. Luego en el siguiente punto, miro más allá. Se que tengo q recolectar nuevas fuentes de info. Cada que vaya a comprar harina poner en un excel, manejar el inventario. Volver a iterar las métricas de negocio, las q no tenga priorizadas.</v>
+        <v/>
       </c>
       <c r="F21" s="12" t="str">
         <f>IFERROR(VLOOKUP($C21,Matriz!$A:$F,VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+F$1,0),"")</f>
-        <v xml:space="preserve">En esta etapa se recomienda tecnificar la generación de informes, buscando disminuir al máximo los tiempos o actividades para generar los indicadores. Siempre teniendo en cuenta que primero cumpla con las siguientes recomendaciones:
-1. Garantice que los indicadores que va a optimizar sí estén aportando al desarrollo de su negocio.
-2. Garantice que la calidad de los datos es la adecuada, si no lo es, revise el punto 1 del nivel de novato.
-3. Eleve el nivel del indicador, ya no sólo piense en que este le debe mostrar un resultado, sino en lo posible coloque una meta o un comparativo, así mismo, defina qué gráfica/tabla le va a permitir tomar las decisiones que necesita de manera más rápida, también defina la periodicidad con la que va a revisar cada indicador.
-Una vez tenga los puntos previos garantizados, trabaje usted o apóyese en alguien experto en excel, para optimizar al máximo la generación de los informes.
-Ejemplo: Los primeros indicadores se generaron cruzando excel, ahora se puede crear una macro para demorarse menos tiempo, puede tener una pestaña inciial con las gráficas gerenciales que definió, así tendrá a la mano la información en un tiempo menor y con menos esfuerzo. 
-</v>
+        <v/>
       </c>
       <c r="G21" s="12" t="str">
         <f>IFERROR(VLOOKUP($C21,Matriz!$A:$F,VLOOKUP(B21,'Diagnóstico de Preparación'!E:F,2,0)+G$1,0),"")</f>
-        <v xml:space="preserve">Al encontrarse la empresa en un nivel de madurez avanzado se recomienda:
-1. Si cuenta con fuentes de información tecnificadas, en otras palabras, con sistemas de información donde tiene registrada los datos, extraiga de manera directa lo requerido para los indicadores, así tendrá siempre información oportuna.
-2. Si genera valor a su negocio, incorpore prácticas de analítica predictiva. Puede ser a través de la incorporación de software comercial existente en el mercado. Es importante identificar cual es el nivel de precisión se espera que tengan las predicciones y qué tanto riesgo puede asumir la empresa al incorporar modelos de este tipo. Se recomienda que inicie con un modelo, explorarlo y afinarlo con base en el uso y resultados que arroje.
-Ejemplos empresa de empanadas: predecir cuándo debe realizar un pedido y en qué cantidades con base en el mes del año, partiendo de la premisa que previamente ya se tiene claro cómo se comporta la demanda del producto.
-</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
       <c r="D24" s="22" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+D$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Inicial</v>
+        <v/>
       </c>
       <c r="E24" s="23" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+E$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Novato</v>
+        <v/>
       </c>
       <c r="F24" s="24" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+F$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Competente</v>
+        <v/>
       </c>
       <c r="G24" s="25" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+G$1,Variables!$Q:$R,2,0),""))</f>
-        <v>Avanzado</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:7" ht="409.5" customHeight="1">
       <c r="A25" s="10" t="str">
         <f>IF(C1="NM","",IFERROR(VLOOKUP(B25,'Diagnóstico de Preparación'!H:I,2,0),""))</f>
-        <v>Procesos</v>
+        <v/>
       </c>
       <c r="B25" s="10">
         <v>6</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" t="e">
         <f>CONCATENATE($C$1,VLOOKUP(A25,Variables!H:I,2,0))</f>
-        <v>M6</v>
+        <v>#N/A</v>
       </c>
       <c r="D25" s="12" t="str">
         <f>IFERROR(VLOOKUP($C25,Matriz!$A:$F,VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+D$1,0),"")</f>
-        <v xml:space="preserve">En este nivel de madurez para la dimensión de procesos se recomienda:
-1. Identifique cuáles de los procesos que se hacen en su empresa son manuales y en cuáles intervienen distintas personas para generar un producto o servicio.
-2. Comience a generar métricas de estos procesos como tiempo que toma elaborar un producto, cantidad de desperdicios generados, tiempo que pasa la materia prima antes de ser recibida por el área encargada, entre otras. Estas métricas pueden ser tomadas inicialmente en papel o en hojas de cálculo de excel. El objetivo de este punto es generar indicadores y determinar la capacidad de su equipo para cada proceso.
-3. Al tener datos cuantificables sobre sus procesos, puede realizar análisis que le permitan tomar algunas decisiones. Ejemplo, para un proceso de producción puede identificar si las máquinas trabajaron bien, si hubo interrupciones en la producción por mantenimientos a las mismas, si tuvo personal de su equipo de trabajo que estuvo por fuera (permisos, incapacidades, vacaciones), si los materiales llegaron en buena calidad o estaban defectuosos. Tener esta información le permitirá identificar cuáles son los factores que intervienen y  son candidatos de mejorar.
-4. Una vez que conoce datos concretos sobre la capacidad de sus procesos, identifique a donde quiere llegar, por ejemplo: Es posible que quiera incremenar la producción, tener mayor visibilidad en el mercado,  mejorar el tiempo de respuesta en sus servicios o mejorar la calidad del producto.
-5. Seleccione máximo dos objetivos que quiere lograr y realice búsquedas en internet (si no sabe como hacerlo puede pedirle a alguien que le oriente en este paso) para identificar si existen soluciones tecnológicas diseñadas para resolver el problema que usted quiere resolver. Algunas búsquedas que puede realizar por ejemplo son: Sistemas para gestión de pedidos, herramientas tecnológica para gestión de inventarios, herramientas de automatización de flujos de trabajo (BPM).
-6. La oferta en el mercado suele ser amplia, vea videos sobre cómo funcionan esas herramientas, infórmese sobre las que le llaman la atención.
-7. Solicite sesiones de demostración y asesoría de algunos fabricantes para que tenga un contexto aterrizado antes de tomar alguna decisión.
-</v>
+        <v/>
       </c>
       <c r="E25" s="12" t="str">
         <f>IFERROR(VLOOKUP($C25,Matriz!$A:$F,VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+E$1,0),"")</f>
-        <v>1. Genere un inventario de los procesos de su empresa y priorice aquellos que son los requeridos para generar ingresos.
-2. Investigue si existen herramientas tecnológicas que le permitan sistematizar cada proceso de la lista anterior.
-(Ejemplo, gestión de pedidos, gestión de inventarios, gestión contable, gestión documental,  herramientas de automatización de flujos de trabajo (BPM), o herramientas de automatización robótica de procesos conocida como RPA, busque ejemplos en alguna herramienta soportada por inteligencia artificial como ChatGPT, entre otros). La oferta en el mercado suele ser amplia, busque cual de las soluciones existentes se puede adaptar mejor de acuerdo con sus necesidades y presupuesto. 
-Solicite sesiones de demostración y asesoría del fabricante para que tenga un contexto aterrizado antes de tomar alguna decisión. 
-3. En caso de que No encuentre que exista una herramienta tecnológica para algún proceso, seleccione uno que considere relevante para buscar iniciativas de sistematización.
-Puede apoyarse buscando sobre Herramientas que no implican desarrollar software, conocidas cmo "no code" o "low code" .
-4. Cada iniciativa de sistematización debería tener: nombre de la inciativa, objetivo de negocio, impacto en la generación de ingresos, complejidad de implementación y costo estimado. Si no conoce todos estos valores, puede partir de algunos supuestos iniciales.Tenga en cuenta todos los procesos de su negocio, principalmente los que involucren múltples tareas manuales.
-En esta etapa es posible que el alcance no cubra el proceso completo, identifique partes del proceso que se estén realizando completamente manuales y repita la búsqueda del punto 2.
-Se sugiere que la priorización la realice tomando en cuenta las iniciativas que más impacto le generan a la empresa, con el fin de que seleccione máximo 2 iniciativas que pueda implementar en el corto plazo y con un presupuesto acorde a su flujo de caja. 
-Si lo considera necesario, asesórese de algún experto.
-Defina un responsable de la ejecución de las iniciativas seleccionadas, un tiempo de implementación y un esquema de seguimiento. También defina los indicadores y/o resultados que considera le permitirán medir el éxito de la implementación que va a realizar.
-Ejecute los proyectos, mida los resultados y consolide lecciones aprendidas.</v>
+        <v/>
       </c>
       <c r="F25" s="12" t="str">
         <f>IFERROR(VLOOKUP($C25,Matriz!$A:$F,VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+F$1,0),"")</f>
-        <v>Defina un portafolio de proyectos que le permita automatizar los procesos que considere más relevantes, utilice el mecanismo de priorización tomando como base el impacto para su negocio de cada uno de los procesos, los de mayor impacto se sugiere sean los primeros en evaluar.  Defina un plan de inversión, proyecte el presupuesto y el flujo de caja de su negocio para definir un horizonte de tiempo realista de ejecución, e inicie su proceso de transformación.
-Recuerde siempre consolidar lecciones aprendidas e incorporarlas en los nuevos proyectos, esto le permitirá ganar velocidad en su ejecución y afinar su capacidad de priorización y evaluación del éxito. No realice planeaciones de más de dos años, y si su línea de tiempo supera este horizonte, antes de ejecutar proyectos del año 3, repita la priorización de iniciativas puesto que es posible que existan cambios.</v>
+        <v/>
       </c>
       <c r="G25" s="12" t="str">
         <f>IFERROR(VLOOKUP($C25,Matriz!$A:$F,VLOOKUP(B25,'Diagnóstico de Preparación'!E:F,2,0)+G$1,0),"")</f>
-        <v>Siga las recomendaciones del nivel competente, pero esta vez, no piense sólo en automatizar, sino en diferenciar su negocio de la competencia. Apóyese en personal conocedor de nuevas tendencias tecnológicas.
-Explore técnicas de innovación y soluciones de inteligencia artificial. Por ejemplo puede buscar información sobre Smart Factory o internet de las cosas (IoT). Dedique una parte del tiempo de su día en explorar y "cacharrear".  Es posible que en este nivel de madurez los proyectos que surjan sean escalables y donde deban intervenir varias personas o áreas de la empresa, por ejemplo mantenimiento, mercadeo, ventas. Explore técnias de mejora continua para cada uno de los procesos de su empresa.</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2728,14 +2619,16 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.5" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.5" hidden="1" customWidth="1"/>
+    <col min="2" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2758,19 +2651,19 @@
       </c>
       <c r="B2">
         <f>SUMIF('Analítica de Datos'!F:F,calculos!$B$1,'Analítica de Datos'!E:E)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>COUNTIF('Analítica de Datos'!F:F,calculos!$B$1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f>SUMIF('Analítica de Datos'!F:F,calculos!$D$1,'Analítica de Datos'!E:E)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>COUNTIF('Analítica de Datos'!F:F,calculos!$D$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2800,19 +2693,19 @@
       </c>
       <c r="B4">
         <f>SUMIF(Procesos!F:F,calculos!$B$1,Procesos!E:E)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>COUNTIF(Procesos!F:F,calculos!$B$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f>SUMIF(Procesos!F:F,calculos!$D$1,Procesos!E:E)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f>COUNTIF(Procesos!F:F,calculos!$D$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2829,11 +2722,11 @@
       </c>
       <c r="D5">
         <f>SUMIF('Visión y Estrategia'!F:F,calculos!$D$1,'Visión y Estrategia'!E:E)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f>COUNTIF('Visión y Estrategia'!F:F,calculos!$D$1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2842,19 +2735,19 @@
       </c>
       <c r="B6">
         <f>SUMIF(Omnicanalidad!F:F,calculos!$B$1,Omnicanalidad!E:E)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>COUNTIF(Omnicanalidad!F:F,calculos!$B$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>SUMIF(Omnicanalidad!F:F,calculos!$D$1,Omnicanalidad!E:E)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>COUNTIF(Omnicanalidad!F:F,calculos!$D$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2863,19 +2756,19 @@
       </c>
       <c r="B7">
         <f>SUMIF(Digitalización!F:F,calculos!$B$1,Digitalización!E:E)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>COUNTIF(Digitalización!F:F,calculos!$B$1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f>SUMIF(Digitalización!F:F,calculos!$D$1,Digitalización!E:E)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f>COUNTIF(Digitalización!F:F,calculos!$D$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2884,19 +2777,19 @@
       </c>
       <c r="B8">
         <f>SUM(B2:B7)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>SUM(C2:C7)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>SUM(D2:D7)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f>SUM(E2:E7)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2905,11 +2798,11 @@
       </c>
       <c r="B9">
         <f>IFERROR(B8/C8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f>IFERROR(D8/E8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2918,19 +2811,19 @@
       </c>
       <c r="B10">
         <f>IF(B9&gt;=4.8,3,IF(AND(B9&gt;=3.4,B9&lt;4.8),2,IF(B9&lt;3.4,1,"error")))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f>IF(D9&gt;=4.6,3,IF(AND(D9&gt;=3,D9&lt;4.6),2,IF(D9&lt;3,1,"error")))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f>((B10*B11)+(D10*D11))*2</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G10" t="str">
         <f>IF(E16="",IF(E17="",IF(E18="",IF(E19="",IF(E20="","Pendiente",E20),E19),E18),E17),E16)</f>
-        <v>Muy motivado</v>
+        <v>No motivado</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2955,7 +2848,7 @@
       </c>
       <c r="E16" t="str">
         <f>IF(F10&gt;=F16,I16,"")</f>
-        <v>Muy motivado</v>
+        <v/>
       </c>
       <c r="F16">
         <v>5.1999999999999993</v>
@@ -3045,7 +2938,7 @@
       </c>
       <c r="E20" t="str">
         <f>IF(AND($F$10&gt;=F20,$F$10&lt;F19),I20,"")</f>
-        <v/>
+        <v>No motivado</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -3077,6 +2970,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="RskcxzRPG3GIVTWRUayvWtmj2YqHdMkwfrVz5OV1yg1cSKL9YxdDn/xsM2zXbxskbK56gc0ambYX47RCFfEWzQ==" saltValue="20T04/o5vif9UHZUo8TN7w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3086,13 +2980,14 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView topLeftCell="W2" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="22" max="22" width="42" customWidth="1"/>
+    <col min="1" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="42" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -3303,6 +3198,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="bxF2r0rdRK2qCOUrVnb5x4harN30AHWkH1QiZI8uJzpP3gr0X6js657bjASPiMaQLSk8QLVYjIvCkROzF1oAew==" saltValue="Q6bmIhPQPrBE6y2tejJiUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3312,8 +3208,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3331,148 +3227,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1"/>
     <row r="4" spans="1:9" ht="47.25" customHeight="1">
-      <c r="A4" s="56">
+      <c r="A4" s="57">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="57">
-        <v>1</v>
+      <c r="C4" s="61"/>
+      <c r="D4" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <f>IFERROR(6-D4,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IF(E4=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="e">
         <f>SUMIF(F:F,H4,E:E)/COUNTIF(F:F,H4)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="157" customHeight="1" thickBot="1">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="e">
         <f>SUMIF(F:F,H5,E:E)/COUNTIF(F:F,H5)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1"/>
     <row r="8" spans="1:9" ht="66.75" customHeight="1">
-      <c r="A8" s="56">
+      <c r="A8" s="57">
         <v>2</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="57">
-        <v>5</v>
+      <c r="C8" s="61"/>
+      <c r="D8" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <f>IF(D8="Seleccione una respuesta",0,D8)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(E8=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" ht="157.5" customHeight="1" thickBot="1">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1"/>
     <row r="12" spans="1:9" ht="48" customHeight="1">
-      <c r="A12" s="56">
+      <c r="A12" s="57">
         <v>3</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="57">
-        <v>1</v>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E12">
         <f>IFERROR(6-D12,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(E12=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="129" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
     </row>
     <row r="15" spans="1:9" ht="16" thickBot="1"/>
     <row r="16" spans="1:9" ht="34.5" customHeight="1">
-      <c r="A16" s="56">
+      <c r="A16" s="57">
         <v>4</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="57">
-        <v>1</v>
+      <c r="C16" s="63"/>
+      <c r="D16" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E16">
         <f>IFERROR(6-D16,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>IF(E16=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:4" ht="127.5" customHeight="1" thickBot="1">
-      <c r="A17" s="56"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3512,8 +3408,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3530,18 +3426,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:14" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="17"/>
       <c r="M2" s="13"/>
       <c r="N2" t="s">
@@ -3549,10 +3445,10 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" hidden="1">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
@@ -3571,30 +3467,30 @@
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1">
-      <c r="A6" s="56">
+      <c r="A6" s="57">
         <v>1</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="57">
-        <v>1</v>
+      <c r="C6" s="61"/>
+      <c r="D6" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E6">
         <f>IFERROR(6-D6,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>IF(E6=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="e">
         <f>SUMIF(F:F,H6,E:E)/COUNTIF(F:F,H6)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M6" s="15"/>
       <c r="N6" t="s">
@@ -3602,18 +3498,18 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="161" thickBot="1">
-      <c r="A7" s="56"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="59"/>
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="e">
         <f>SUMIF(F:F,H7,E:E)/COUNTIF(F:F,H7)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M7" s="16"/>
       <c r="N7" t="s">
@@ -3627,32 +3523,32 @@
       <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1">
-      <c r="A10" s="56">
+      <c r="A10" s="57">
         <v>2</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="57">
-        <v>1</v>
+      <c r="C10" s="61"/>
+      <c r="D10" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E10">
         <f>IFERROR(6-D10,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>IF(E10=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:14" ht="129" thickBot="1">
-      <c r="A11" s="56"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="58"/>
+      <c r="D11" s="59"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1"/>
@@ -3661,32 +3557,32 @@
       <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="22" customHeight="1">
-      <c r="A14" s="56">
+      <c r="A14" s="57">
         <v>3</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="57">
-        <v>1</v>
+      <c r="C14" s="61"/>
+      <c r="D14" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E14">
         <f>IFERROR(6-D14,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>IF(E14=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:14" ht="81" thickBot="1">
-      <c r="A15" s="56"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="58"/>
+      <c r="D15" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3730,8 +3626,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:K1048576"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3742,60 +3638,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1"/>
     <row r="4" spans="1:9">
-      <c r="A4" s="56">
+      <c r="A4" s="57">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="57">
-        <v>1</v>
+      <c r="C4" s="61"/>
+      <c r="D4" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <f>IFERROR(6-D4,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IF(E4=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="e">
         <f>SUMIF(F:F,H4,E:E)/COUNTIF(F:F,H4)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="97" thickBot="1">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="e">
         <f>SUMIF(F:F,H5,E:E)/COUNTIF(F:F,H5)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3805,32 +3701,32 @@
       <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="56">
+      <c r="A8" s="57">
         <v>2</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="57">
-        <v>1</v>
+      <c r="C8" s="61"/>
+      <c r="D8" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <f>IFERROR(6-D8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(E8=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" ht="113" thickBot="1">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1"/>
@@ -3839,32 +3735,32 @@
       <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="56">
+      <c r="A12" s="57">
         <v>3</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="57">
-        <v>1</v>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E12">
         <f>IFERROR(6-D12,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(E12=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="97" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3901,8 +3797,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:O1048576"/>
+    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3914,39 +3810,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:11" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="F2" s="68"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="16" thickBot="1"/>
     <row r="4" spans="1:11" ht="30" customHeight="1">
-      <c r="A4" s="56">
+      <c r="A4" s="57">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="57">
-        <v>1</v>
+      <c r="C4" s="61"/>
+      <c r="D4" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <f>IFERROR(6-D4,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IF(E4=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -3957,77 +3853,77 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="97" thickBot="1">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="e">
         <f>SUMIF(F:F,H5,E:E)/COUNTIF(F:F,H5)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16" thickBot="1"/>
     <row r="8" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A8" s="56">
+      <c r="A8" s="57">
         <v>2</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="57">
-        <v>1</v>
+      <c r="C8" s="61"/>
+      <c r="D8" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <f>IFERROR(6-D8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(E8=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:11" ht="97" thickBot="1">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
     </row>
     <row r="11" spans="1:11" ht="16" thickBot="1"/>
     <row r="12" spans="1:11">
-      <c r="A12" s="56">
+      <c r="A12" s="57">
         <v>3</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="57">
-        <v>1</v>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E12">
         <f>IFERROR(6-D12,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(E12=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:11" ht="145" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
       <c r="J13" t="s">
         <v>125</v>
       </c>
@@ -4037,20 +3933,20 @@
     </row>
     <row r="15" spans="1:11" ht="16" thickBot="1"/>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="57">
-        <v>1</v>
+      <c r="C16" s="61"/>
+      <c r="D16" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E16">
         <f>IFERROR(6-D16,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>IF(E16=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:10" ht="145" thickBot="1">
@@ -4061,13 +3957,18 @@
       <c r="C17" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="59"/>
       <c r="J17" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="B4:C4"/>
@@ -4076,11 +3977,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4103,8 +3999,8 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:L1048576"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4115,60 +4011,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1"/>
     <row r="4" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A4" s="56">
+      <c r="A4" s="57">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="57">
-        <v>1</v>
+      <c r="C4" s="61"/>
+      <c r="D4" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <f>IFERROR(6-D4,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IF(E4=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="e">
         <f>SUMIF(F:F,H4,E:E)/COUNTIF(F:F,H4)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="129" thickBot="1">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="e">
         <f>SUMIF(F:F,H5,E:E)/COUNTIF(F:F,H5)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4178,32 +4074,32 @@
       <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="56">
+      <c r="A8" s="57">
         <v>2</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="57">
-        <v>1</v>
+      <c r="C8" s="61"/>
+      <c r="D8" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <f>IFERROR(6-D8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(E8=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" ht="97" thickBot="1">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1"/>
@@ -4212,32 +4108,32 @@
       <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="56">
+      <c r="A12" s="57">
         <v>3</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="57">
-        <v>1</v>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E12">
         <f>IFERROR(6-D12,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(E12=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="113" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4274,8 +4170,8 @@
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4292,139 +4188,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:9" ht="29">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1"/>
     <row r="4" spans="1:9">
-      <c r="A4" s="56">
+      <c r="A4" s="57">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="57">
-        <v>1</v>
+      <c r="C4" s="61"/>
+      <c r="D4" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <f>IFERROR(6-D4,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IF(E4=0,"","I")</f>
-        <v>I</v>
+        <v/>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="e">
         <f>SUMIF(F:F,H4,E:E)/COUNTIF(F:F,H4)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="97" thickBot="1">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="e">
         <f>SUMIF(F:F,H5,E:E)/COUNTIF(F:F,H5)</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1"/>
     <row r="8" spans="1:9">
-      <c r="A8" s="56">
+      <c r="A8" s="57">
         <v>2</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="57">
-        <v>1</v>
+      <c r="C8" s="61"/>
+      <c r="D8" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
         <f>IFERROR(6-D8,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(E8=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" ht="129" thickBot="1">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="59"/>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1"/>
     <row r="12" spans="1:9">
-      <c r="A12" s="56">
+      <c r="A12" s="57">
         <v>3</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="57">
-        <v>1</v>
+      <c r="C12" s="61"/>
+      <c r="D12" s="58" t="s">
+        <v>9</v>
       </c>
       <c r="E12">
         <f>IFERROR(6-D12,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(E12=0,"","U")</f>
-        <v>U</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="161" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="59"/>
     </row>
     <row r="15" spans="1:9" ht="16" thickBot="1"/>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A16" s="63">
+      <c r="A16" s="64">
         <v>4</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="60"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="61"/>
     </row>
     <row r="17" spans="1:4" s="6" customFormat="1" ht="154" customHeight="1" thickBot="1">
-      <c r="A17" s="63"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="45"/>
       <c r="C17" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="47">
-        <v>1</v>
+      <c r="D17" s="47" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4432,11 +4328,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B4:C4"/>
@@ -4445,6 +4336,11 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <conditionalFormatting sqref="B16:B17">
     <cfRule type="expression" dxfId="7" priority="2">
@@ -4496,24 +4392,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="29" customHeight="1">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="42"/>
       <c r="G1" t="str">
         <f>'Matriz de Recomendaciones'!C1</f>
-        <v>M</v>
+        <v>NM</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
       <c r="D2" s="42"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="42"/>
     </row>
     <row r="4" spans="2:10"/>
@@ -4536,9 +4432,9 @@
         <f>VLOOKUP(C5,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="str">
         <f t="shared" ref="G5:G10" si="1">IF($G$1="PM",IF(F5&gt;=2,1,2),IF($G$1="M",1,""))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H5">
         <f>IF(G5=2,0,1)</f>
@@ -4572,9 +4468,9 @@
         <f>VLOOKUP(C6,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H6">
         <f>IF(G6=2,H5,H5+1)</f>
@@ -4608,9 +4504,9 @@
         <f>VLOOKUP(C7,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H7">
         <f>IF(G7=2,H6,H6+1)</f>
@@ -4640,9 +4536,9 @@
         <f>VLOOKUP(C8,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H8">
         <f>IF(G8=2,H7,H7+1)</f>
@@ -4672,9 +4568,9 @@
         <f>VLOOKUP(C9,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H9">
         <f>IF(G9=2,H8,H8+1)</f>
@@ -4704,9 +4600,9 @@
         <f>VLOOKUP(C10,Variables!K:L,2,0)</f>
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="H10">
         <f>IF(G10=2,H9,H9+1)</f>

</xml_diff>